<commit_message>
adding transaction to Q
</commit_message>
<xml_diff>
--- a/JAR-StockManager/Data/Config.xlsx
+++ b/JAR-StockManager/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature_Workspace\Jar-P2\JAR-StockManager\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\revature-workspace\Jar-P2\JAR-StockManager\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2CB512-E22C-4057-9F94-881604B9B12B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA78251-5321-4BF6-B8D7-5668E446B44C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="675" yWindow="1095" windowWidth="27420" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -90,19 +90,11 @@
     <t>Framework</t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -133,7 +125,10 @@
     <t>OutlookCredentials</t>
   </si>
   <si>
-    <t>OutlookCredential</t>
+    <t>StockQueue</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
   </si>
 </sst>
 </file>
@@ -519,7 +514,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -566,16 +561,23 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
         <v>20</v>
@@ -584,19 +586,19 @@
         <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
         <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1653,7 +1655,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1677,7 +1679,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1699,7 +1701,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1710,7 +1712,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1721,7 +1723,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2711,8 +2713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2758,12 +2760,8 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>34</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="5"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
everything but the wrap up done
</commit_message>
<xml_diff>
--- a/JAR-StockManager/Data/Config.xlsx
+++ b/JAR-StockManager/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\revature-workspace\Jar-P2\JAR-StockManager\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rache\OneDrive\Documents\UiPath\Jar-P2\JAR-StockManager\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA78251-5321-4BF6-B8D7-5668E446B44C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6F83B4-6D3D-4A12-9004-0397B2813C00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>Counter</t>
+  </si>
+  <si>
+    <t>used to increment the row of the stock data excel file</t>
   </si>
 </sst>
 </file>
@@ -514,15 +520,15 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -578,7 +584,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="30">
+    <row r="4" spans="1:26" ht="28.8">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -601,7 +607,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1605,12 +1621,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1647,7 +1663,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2717,12 +2733,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
everything besides embeded html images
</commit_message>
<xml_diff>
--- a/JAR-StockManager/Data/Config.xlsx
+++ b/JAR-StockManager/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rache\OneDrive\Documents\UiPath\Jar-P2\JAR-StockManager\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\revature-workspace\Jar-P2\Jar-P2\JAR-StockManager\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6F83B4-6D3D-4A12-9004-0397B2813C00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A2C014-CD62-4BA6-A34C-BBAC32014FE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -520,15 +520,15 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -584,7 +584,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="28.8">
+    <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1621,12 +1621,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1663,7 +1663,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2733,12 +2733,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>